<commit_message>
Change code to accomondate Assemblyline change
make the access node flexible.
smart detect file type for csv and txt as well as other entity, automatically fill in MIME types.
add maintnance and license column in Excel workbook.
</commit_message>
<xml_diff>
--- a/Metadata/Metadata.xlsx
+++ b/Metadata/Metadata.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lkui/Desktop/Excel_to_EML_Assembly/Metadata/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lkui/Documents/GitHub/Excel-to-EML/Metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4B28F13-1101-284E-AC7B-B6CA281011EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCD49227-1B8B-4A4A-B272-49D2A5F119C0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17280" yWindow="3540" windowWidth="27320" windowHeight="20140" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1560" yWindow="6460" windowWidth="29520" windowHeight="12340" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
@@ -403,6 +403,39 @@
     <author>LK</author>
   </authors>
   <commentList>
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{C9D1FE79-5BAC-B742-A0BE-273D758927DA}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>LK:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Common styles of access node and headspace: LTER, EDI, KNB, and ADC</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="C1" authorId="0" shapeId="0" xr:uid="{533A845F-9816-CC4C-83D7-AF4A606E2F36}">
       <text>
         <r>
@@ -432,7 +465,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>This is for "Principal" access in the EML</t>
+          <t>This is for EML that requires userid</t>
         </r>
       </text>
     </comment>
@@ -441,7 +474,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2268" uniqueCount="1190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2273" uniqueCount="1196">
   <si>
     <t>dataTable</t>
   </si>
@@ -3851,9 +3884,6 @@
     <t>field site</t>
   </si>
   <si>
-    <t>stellalab</t>
-  </si>
-  <si>
     <t>plantid</t>
   </si>
   <si>
@@ -3899,12 +3929,6 @@
     <t>giant kelp</t>
   </si>
   <si>
-    <t>PISCO</t>
-  </si>
-  <si>
-    <t>NSF0000</t>
-  </si>
-  <si>
     <t>Giant kelp</t>
   </si>
   <si>
@@ -3950,9 +3974,6 @@
     <t>01234</t>
   </si>
   <si>
-    <t>other.domain.ID</t>
-  </si>
-  <si>
     <t>project xml</t>
   </si>
   <si>
@@ -4011,6 +4032,36 @@
   </si>
   <si>
     <t>pdf_method.pdf</t>
+  </si>
+  <si>
+    <t>maintenance</t>
+  </si>
+  <si>
+    <t>completed</t>
+  </si>
+  <si>
+    <t>Ongoing collection with update quarterly</t>
+  </si>
+  <si>
+    <t>CCBY</t>
+  </si>
+  <si>
+    <t>CC0</t>
+  </si>
+  <si>
+    <t>intellectual_right</t>
+  </si>
+  <si>
+    <t>other.domain</t>
+  </si>
+  <si>
+    <t>PISCO funding</t>
+  </si>
+  <si>
+    <t>NSF0000000</t>
+  </si>
+  <si>
+    <t>KNB</t>
   </si>
 </sst>
 </file>
@@ -4021,7 +4072,7 @@
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
     <numFmt numFmtId="165" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -4056,6 +4107,13 @@
       <name val="Arial Unicode MS"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -4078,7 +4136,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -4089,6 +4147,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -4370,10 +4429,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:H1048576"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4385,12 +4444,14 @@
     <col min="5" max="5" width="15.83203125" style="2" customWidth="1"/>
     <col min="6" max="6" width="17.6640625" style="2" customWidth="1"/>
     <col min="7" max="7" width="11.6640625" style="2" customWidth="1"/>
-    <col min="9" max="9" width="10.1640625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="17.1640625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="17.6640625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="16.5" style="2" customWidth="1"/>
+    <col min="10" max="10" width="10.1640625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="17.1640625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="17.6640625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="12.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>843</v>
       </c>
@@ -4404,28 +4465,31 @@
         <v>866</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>1138</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>1139</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>1140</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>867</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>1186</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>1115</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>1141</v>
-      </c>
       <c r="J1" s="1" t="s">
-        <v>1143</v>
+        <v>1140</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>1142</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L1" s="1" t="s">
+        <v>1141</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>99</v>
       </c>
@@ -4436,7 +4500,7 @@
         <v>2</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="E2" s="2">
         <v>41460</v>
@@ -4447,53 +4511,62 @@
       <c r="G2" s="2">
         <v>43328</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="2" t="s">
+        <v>1187</v>
+      </c>
+      <c r="I2" t="s">
         <v>1117</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>1121</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="K2" s="1" t="s">
+        <v>1145</v>
+      </c>
+      <c r="L2" s="1" t="s">
         <v>1146</v>
       </c>
-      <c r="K2" s="1" t="s">
-        <v>1147</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>100</v>
       </c>
       <c r="B3" t="s">
-        <v>1169</v>
+        <v>1192</v>
       </c>
       <c r="C3">
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="E3" s="2">
         <v>39448</v>
       </c>
       <c r="F3" s="2">
-        <v>43831</v>
+        <v>43159</v>
       </c>
       <c r="G3" s="2">
-        <v>43985</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>1144</v>
+        <v>44040</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>1188</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>1119</v>
+        <v>1143</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>1152</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>1153</v>
-      </c>
+        <v>1120</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>1193</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>1194</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="H11" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4505,8 +4578,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:S31"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4831,9 +4904,6 @@
       <c r="L7" t="s">
         <v>153</v>
       </c>
-      <c r="M7" t="s">
-        <v>26</v>
-      </c>
       <c r="N7" t="s">
         <v>155</v>
       </c>
@@ -5582,7 +5652,7 @@
         <v>92</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>1178</v>
+        <v>1174</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>64</v>
@@ -5611,7 +5681,7 @@
         <v>93</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>1179</v>
+        <v>1175</v>
       </c>
       <c r="D26" s="3" t="s">
         <v>107</v>
@@ -5634,19 +5704,19 @@
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>1175</v>
+        <v>1171</v>
       </c>
       <c r="B27" t="s">
-        <v>1177</v>
+        <v>1173</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>1180</v>
+        <v>1176</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>1175</v>
+        <v>1171</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>1176</v>
+        <v>1172</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>137</v>
@@ -5658,7 +5728,7 @@
         <v>149</v>
       </c>
       <c r="R27" s="1" t="s">
-        <v>1176</v>
+        <v>1172</v>
       </c>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.2">
@@ -5669,7 +5739,7 @@
         <v>75</v>
       </c>
       <c r="C28" t="s">
-        <v>1186</v>
+        <v>1182</v>
       </c>
       <c r="D28" s="3" t="s">
         <v>96</v>
@@ -5687,7 +5757,7 @@
         <v>149</v>
       </c>
       <c r="R28" t="s">
-        <v>1185</v>
+        <v>1181</v>
       </c>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.2">
@@ -5698,7 +5768,7 @@
         <v>76</v>
       </c>
       <c r="C29" t="s">
-        <v>1183</v>
+        <v>1179</v>
       </c>
       <c r="D29" s="3" t="s">
         <v>103</v>
@@ -5716,7 +5786,7 @@
         <v>149</v>
       </c>
       <c r="R29" t="s">
-        <v>1184</v>
+        <v>1180</v>
       </c>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.2">
@@ -5727,7 +5797,7 @@
         <v>77</v>
       </c>
       <c r="C30" t="s">
-        <v>1187</v>
+        <v>1183</v>
       </c>
       <c r="D30" s="3" t="s">
         <v>104</v>
@@ -5745,7 +5815,7 @@
         <v>149</v>
       </c>
       <c r="R30" t="s">
-        <v>1173</v>
+        <v>1169</v>
       </c>
     </row>
     <row r="31" spans="1:19" ht="16" x14ac:dyDescent="0.25">
@@ -5756,7 +5826,7 @@
         <v>78</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>1182</v>
+        <v>1178</v>
       </c>
       <c r="D31" s="3" t="s">
         <v>105</v>
@@ -5774,7 +5844,7 @@
         <v>149</v>
       </c>
       <c r="R31" t="s">
-        <v>1181</v>
+        <v>1177</v>
       </c>
     </row>
   </sheetData>
@@ -12531,7 +12601,7 @@
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -12588,7 +12658,7 @@
       <c r="E2" t="s">
         <v>1057</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G2" s="4" t="s">
@@ -12614,14 +12684,14 @@
       <c r="E3" t="s">
         <v>1056</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>983</v>
       </c>
       <c r="H3" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
@@ -12664,7 +12734,7 @@
         <v>1134</v>
       </c>
       <c r="E5" t="s">
-        <v>1174</v>
+        <v>1170</v>
       </c>
       <c r="F5" t="s">
         <v>20</v>
@@ -12673,7 +12743,7 @@
         <v>983</v>
       </c>
       <c r="H5" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
     </row>
     <row r="6" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -12687,10 +12757,10 @@
         <v>1133</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>1170</v>
+        <v>1166</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>1171</v>
+        <v>1167</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>64</v>
@@ -12699,7 +12769,7 @@
         <v>983</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>1172</v>
+        <v>1168</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
@@ -12713,17 +12783,17 @@
         <v>0</v>
       </c>
       <c r="D7" t="s">
-        <v>1154</v>
+        <v>1151</v>
       </c>
       <c r="E7" t="s">
-        <v>1154</v>
-      </c>
-      <c r="F7" s="1" t="s">
+        <v>1151</v>
+      </c>
+      <c r="F7" s="10" t="s">
         <v>1</v>
       </c>
       <c r="G7" s="4"/>
       <c r="H7" s="7" t="s">
-        <v>1155</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
@@ -12737,16 +12807,19 @@
         <v>1133</v>
       </c>
       <c r="D8" t="s">
-        <v>1175</v>
+        <v>1171</v>
       </c>
       <c r="E8" t="s">
-        <v>1188</v>
+        <v>1184</v>
       </c>
       <c r="F8" t="s">
-        <v>1175</v>
+        <v>1171</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>983</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>1189</v>
+        <v>1185</v>
       </c>
     </row>
   </sheetData>
@@ -12757,28 +12830,29 @@
     <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="need a matching file type" sqref="F1" xr:uid="{4380E1FC-047D-F54D-93BE-FA4ACEBAE2DB}"/>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="G4" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
-    <hyperlink ref="G5" r:id="rId2" xr:uid="{09C412E3-B952-0940-B490-0629BEBC777E}"/>
-    <hyperlink ref="G3" r:id="rId3" xr:uid="{4B206A9D-228D-AB48-9EDD-F070AC8345D5}"/>
-    <hyperlink ref="G6" r:id="rId4" xr:uid="{1820F47D-6892-C445-BBF9-91A8E2B7AB60}"/>
-    <hyperlink ref="G2" r:id="rId5" xr:uid="{35E5FA29-C390-234D-A8AB-F8B9BF153B1D}"/>
+    <hyperlink ref="G6" r:id="rId1" xr:uid="{1820F47D-6892-C445-BBF9-91A8E2B7AB60}"/>
+    <hyperlink ref="G8" r:id="rId2" xr:uid="{73FFD213-9607-F74F-BE02-74F011F1952C}"/>
+    <hyperlink ref="G5" r:id="rId3" xr:uid="{A83409B4-4645-5846-B99A-99F88076AE21}"/>
+    <hyperlink ref="G2" r:id="rId4" xr:uid="{DDDE8A45-DF58-F340-9B0B-4E4D6A2EAF52}"/>
+    <hyperlink ref="G3" r:id="rId5" xr:uid="{E2D49E67-5020-5F42-BA28-12635309AEF0}"/>
+    <hyperlink ref="G4" r:id="rId6" xr:uid="{E06EA28A-B529-0D4E-B548-E48302CF2170}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId6"/>
+  <legacyDrawing r:id="rId7"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+        <x14:dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="need a matching file type" xr:uid="{D3FC84DB-410B-704A-941B-266D95E2969F}">
+          <x14:formula1>
+            <xm:f>ListFileType!$A$2:$A$86</xm:f>
+          </x14:formula1>
+          <xm:sqref>F2:F6 F8:F1048576</xm:sqref>
+        </x14:dataValidation>
         <x14:dataValidation type="list" errorStyle="warning" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="datasetid doesn't match" promptTitle="Match id in DataSet Sheet" xr:uid="{B9F16F1E-E81A-2B40-AE2F-5B37AF6BEB61}">
           <x14:formula1>
             <xm:f>DataSet!$A:$A</xm:f>
           </x14:formula1>
           <xm:sqref>A1:A1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="need a matching file type" xr:uid="{D3FC84DB-410B-704A-941B-266D95E2969F}">
-          <x14:formula1>
-            <xm:f>ListFileType!$A$2:$A$86</xm:f>
-          </x14:formula1>
-          <xm:sqref>F2:F1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -12790,9 +12864,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:K40"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B15" sqref="B15:B32"/>
+      <selection pane="bottomLeft" activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -12823,7 +12897,7 @@
         <v>1128</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>16</v>
@@ -13613,7 +13687,7 @@
         <v>3</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>984</v>
@@ -13630,7 +13704,7 @@
         <v>3</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>1138</v>
+        <v>1137</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>1014</v>
@@ -13682,16 +13756,16 @@
         <v>1</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>1156</v>
+        <v>1153</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>1156</v>
+        <v>1153</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>1161</v>
+        <v>1158</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>1167</v>
+        <v>1164</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.2">
@@ -13702,10 +13776,10 @@
         <v>1</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>1157</v>
+        <v>1154</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>1157</v>
+        <v>1154</v>
       </c>
       <c r="E37" s="1" t="s">
         <v>1129</v>
@@ -13719,10 +13793,10 @@
         <v>1</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>1158</v>
+        <v>1155</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>1158</v>
+        <v>1155</v>
       </c>
       <c r="E38" s="1" t="s">
         <v>1129</v>
@@ -13736,10 +13810,10 @@
         <v>1</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>1159</v>
+        <v>1156</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>1159</v>
+        <v>1156</v>
       </c>
       <c r="E39" s="1" t="s">
         <v>1130</v>
@@ -13757,7 +13831,7 @@
         <v>-99999</v>
       </c>
       <c r="K39" s="1" t="s">
-        <v>1162</v>
+        <v>1159</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.2">
@@ -13768,10 +13842,10 @@
         <v>1</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>1160</v>
+        <v>1157</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>1160</v>
+        <v>1157</v>
       </c>
       <c r="E40" s="1" t="s">
         <v>1129</v>
@@ -14089,7 +14163,7 @@
         <v>100</v>
       </c>
       <c r="B14" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="C14" t="s">
         <v>14</v>
@@ -14106,7 +14180,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -14267,7 +14341,7 @@
         <v>100</v>
       </c>
       <c r="B4" t="s">
-        <v>1163</v>
+        <v>1160</v>
       </c>
       <c r="C4">
         <v>34</v>
@@ -14416,10 +14490,10 @@
         <v>35</v>
       </c>
       <c r="M3" s="8" t="s">
-        <v>1166</v>
+        <v>1163</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>1164</v>
+        <v>1161</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
@@ -14457,7 +14531,7 @@
         <v>37</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>1164</v>
+        <v>1161</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
@@ -14492,13 +14566,13 @@
         <v>34</v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>1168</v>
+        <v>1165</v>
       </c>
       <c r="M5" s="8" t="s">
-        <v>1165</v>
+        <v>1162</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>1164</v>
+        <v>1161</v>
       </c>
     </row>
   </sheetData>
@@ -14512,18 +14586,20 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88B25934-9280-524E-B624-293E63FB208B}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="16384" width="10.83203125" style="6"/>
+    <col min="1" max="3" width="10.83203125" style="6"/>
+    <col min="4" max="4" width="15.83203125" style="6" customWidth="1"/>
+    <col min="5" max="16384" width="10.83203125" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>1115</v>
       </c>
@@ -14533,8 +14609,11 @@
       <c r="C1" s="6" t="s">
         <v>1127</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D1" s="6" t="s">
+        <v>1191</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
         <v>1117</v>
       </c>
@@ -14544,19 +14623,27 @@
       <c r="C2" s="6" t="s">
         <v>1120</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D2" s="6" t="s">
+        <v>1189</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>1152</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>1136</v>
+        <v>1195</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>1190</v>
       </c>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576" xr:uid="{2B1995F4-CDEB-7E4C-9CEC-2CDAF6E0DAD0}">
+      <formula1>"CCBY, CC0"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>

</xml_diff>